<commit_message>
autosize nodes to image
</commit_message>
<xml_diff>
--- a/contents/battle/battle_2/battle_2.xlsx
+++ b/contents/battle/battle_2/battle_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imanol-KS53\Documents\Imanol\Github_projects\InteractiveBook\contents\battle\battle_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121B50BE-22B9-4611-A80B-87AF11EF79BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2912E06E-198E-4992-8067-3ACAA8CE38D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +626,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -646,7 +646,7 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -663,7 +663,7 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -683,7 +683,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -703,7 +703,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -723,7 +723,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -743,7 +743,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -760,7 +760,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -780,7 +780,7 @@
         <v>5</v>
       </c>
       <c r="C10">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -800,7 +800,7 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -820,7 +820,7 @@
         <v>4</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -840,7 +840,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -857,7 +857,7 @@
         <v>8</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -877,7 +877,7 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -897,7 +897,7 @@
         <v>6</v>
       </c>
       <c r="C16">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -917,7 +917,7 @@
         <v>5</v>
       </c>
       <c r="C17">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -937,7 +937,7 @@
         <v>7</v>
       </c>
       <c r="C18">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -957,7 +957,7 @@
         <v>4</v>
       </c>
       <c r="C19">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -977,7 +977,7 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -997,7 +997,7 @@
         <v>5</v>
       </c>
       <c r="C21">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1017,7 +1017,7 @@
         <v>7</v>
       </c>
       <c r="C22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1034,10 +1034,10 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>13.5</v>
+        <v>14.5</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1051,10 +1051,10 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C24">
-        <v>13.5</v>
+        <v>14.5</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1074,7 +1074,7 @@
         <v>5</v>
       </c>
       <c r="C25">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1094,7 +1094,7 @@
         <v>7</v>
       </c>
       <c r="C26">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1114,7 +1114,7 @@
         <v>4</v>
       </c>
       <c r="C27">
-        <v>16.5</v>
+        <v>17.5</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1134,7 +1134,7 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <v>16.5</v>
+        <v>17.5</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1151,7 +1151,7 @@
         <v>8</v>
       </c>
       <c r="C29">
-        <v>16.5</v>
+        <v>17.5</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1171,7 +1171,7 @@
         <v>5</v>
       </c>
       <c r="C30">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1191,7 +1191,7 @@
         <v>7</v>
       </c>
       <c r="C31">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1211,7 +1211,7 @@
         <v>4</v>
       </c>
       <c r="C32">
-        <v>19.5</v>
+        <v>20.5</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1231,7 +1231,7 @@
         <v>6</v>
       </c>
       <c r="C33">
-        <v>19.5</v>
+        <v>20.5</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1248,7 +1248,7 @@
         <v>8</v>
       </c>
       <c r="C34">
-        <v>19.5</v>
+        <v>20.5</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1268,7 +1268,7 @@
         <v>5</v>
       </c>
       <c r="C35">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1288,7 +1288,7 @@
         <v>7</v>
       </c>
       <c r="C36">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1308,7 +1308,7 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="D37">
         <v>7</v>
@@ -1325,7 +1325,7 @@
         <v>2.5</v>
       </c>
       <c r="C38">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -1345,7 +1345,7 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
       <c r="D39">
         <v>7</v>
@@ -1362,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="C40">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D40">
         <v>7</v>
@@ -1379,7 +1379,7 @@
         <v>11</v>
       </c>
       <c r="C41">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="D41">
         <v>7</v>
@@ -1396,7 +1396,7 @@
         <v>9.5</v>
       </c>
       <c r="C42">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1416,7 +1416,7 @@
         <v>12</v>
       </c>
       <c r="C43">
-        <v>10.5</v>
+        <v>11.5</v>
       </c>
       <c r="D43">
         <v>7</v>
@@ -1433,7 +1433,7 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <v>12.75</v>
+        <v>13.75</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -1453,7 +1453,7 @@
         <v>12</v>
       </c>
       <c r="C45">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D45">
         <v>7</v>

</xml_diff>